<commit_message>
name fix + output
</commit_message>
<xml_diff>
--- a/data/xlsx_edit/physrost02.xlsx
+++ b/data/xlsx_edit/physrost02.xlsx
@@ -1165,13 +1165,13 @@
     <t xml:space="preserve">101</t>
   </si>
   <si>
-    <t xml:space="preserve">Indiana U Purdue U Ft Wayne</t>
+    <t xml:space="preserve">Indiana U Purdue U-Ft Wayne</t>
   </si>
   <si>
     <t xml:space="preserve">490</t>
   </si>
   <si>
-    <t xml:space="preserve">Indiana U Purdue U Indpls</t>
+    <t xml:space="preserve">Indiana U Purdue U-Indpls</t>
   </si>
   <si>
     <t xml:space="preserve">Indianapolis-U of</t>
@@ -1192,13 +1192,13 @@
     <t xml:space="preserve">898</t>
   </si>
   <si>
-    <t xml:space="preserve">Purdue U Calumet</t>
+    <t xml:space="preserve">Purdue U-Calumet</t>
   </si>
   <si>
     <t xml:space="preserve">472</t>
   </si>
   <si>
-    <t xml:space="preserve">Purdue U West Lafayette</t>
+    <t xml:space="preserve">Purdue U-West Lafayette</t>
   </si>
   <si>
     <t xml:space="preserve">3676</t>
@@ -4148,14 +4148,14 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A361" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A205" activeCellId="0" sqref="A205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.55"/>

</xml_diff>